<commit_message>
Updated with path based comparison
</commit_message>
<xml_diff>
--- a/samples/idaithalam-excel-apitesting/src/test/resources/virtualan_collection_testcase_6.xlsx
+++ b/samples/idaithalam-excel-apitesting/src/test/resources/virtualan_collection_testcase_6.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -34,9 +34,6 @@
     <t>RequestProcessingType</t>
   </si>
   <si>
-    <t>ResponseByField</t>
-  </si>
-  <si>
     <t>ResponseFile</t>
   </si>
   <si>
@@ -73,13 +70,13 @@
     <t>https://live.virtualandemo.com/api/pets</t>
   </si>
   <si>
-    <t>application/x-www-urlencoded</t>
-  </si>
-  <si>
-    <t>id=100;name=[petName]</t>
-  </si>
-  <si>
-    <t>post-response.json</t>
+    <t>application/x-www-form-urlencoded</t>
+  </si>
+  <si>
+    <t>id=100;name=doggie</t>
+  </si>
+  <si>
+    <t>Accept=application/json</t>
   </si>
   <si>
     <t>POST</t>
@@ -95,7 +92,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -118,6 +115,11 @@
       <color rgb="FF1155CC"/>
       <name val="Inconsolata"/>
     </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF24292E"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -139,7 +141,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -153,6 +155,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -374,10 +379,9 @@
     <col customWidth="1" min="2" max="2" width="18.14"/>
     <col customWidth="1" min="3" max="3" width="176.14"/>
     <col customWidth="1" min="7" max="7" width="21.71"/>
-    <col customWidth="1" min="8" max="8" width="24.29"/>
-    <col customWidth="1" min="10" max="10" width="23.29"/>
-    <col customWidth="1" min="14" max="14" width="49.29"/>
-    <col customWidth="1" min="15" max="15" width="24.29"/>
+    <col customWidth="1" min="9" max="9" width="23.29"/>
+    <col customWidth="1" min="13" max="13" width="49.29"/>
+    <col customWidth="1" min="14" max="14" width="24.29"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -402,7 +406,7 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -428,44 +432,38 @@
       </c>
       <c r="P1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1">
+        <v>415.0</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="M2" s="1">
-        <v>200.0</v>
-      </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Workflow disable feature to enable all testcases
</commit_message>
<xml_diff>
--- a/samples/idaithalam-excel-apitesting/src/test/resources/virtualan_collection_testcase_6.xlsx
+++ b/samples/idaithalam-excel-apitesting/src/test/resources/virtualan_collection_testcase_6.xlsx
@@ -111,11 +111,14 @@
   <si>
     <t>Tags</t>
   </si>
+  <si>
+    <t>PetPost_1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="8" mc:Ignorable="x14ac">
   <numFmts count="8">
     <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);(&quot;$&quot;#,##0)"/>
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red](&quot;$&quot;#,##0)"/>
@@ -401,7 +404,7 @@
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q1" sqref="Q1"/>
+      <selection pane="topLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="14.43" defaultRowHeight="15"/>
@@ -496,9 +499,42 @@
         <v>24</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" s="1">
+        <v>415</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId1"/>
   </hyperlinks>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated wit \r fix
</commit_message>
<xml_diff>
--- a/samples/idaithalam-excel-apitesting/src/test/resources/virtualan_collection_testcase_6.xlsx
+++ b/samples/idaithalam-excel-apitesting/src/test/resources/virtualan_collection_testcase_6.xlsx
@@ -404,7 +404,7 @@
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" sqref="B8"/>
+      <selection pane="topLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="14.43" defaultRowHeight="15"/>
@@ -499,38 +499,6 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3" s="1">
-        <v>415</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>

</xml_diff>